<commit_message>
changes to possession model, added model.py
</commit_message>
<xml_diff>
--- a/DK Salary Optimization Sheets/DKSalaries_11222014_optimization.xlsx
+++ b/DK Salary Optimization Sheets/DKSalaries_11222014_optimization.xlsx
@@ -107,7 +107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1301" uniqueCount="515">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1307" uniqueCount="515">
   <si>
     <t>Position</t>
   </si>
@@ -2224,14 +2224,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="7">
     <dxf>
       <fill>
         <patternFill>
@@ -2559,8 +2552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA328"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T5" sqref="T5"/>
+    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="Z21" sqref="Z21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2647,7 +2640,7 @@
       </c>
       <c r="U1" s="2">
         <f>SUM(K2:K230)</f>
-        <v>256.98366749071795</v>
+        <v>250.79471548920117</v>
       </c>
       <c r="V1" t="s">
         <v>15</v>
@@ -2695,7 +2688,7 @@
         <v>47.922183194688699</v>
       </c>
       <c r="I2" s="4">
-        <f>IF(ISNA(VLOOKUP(B2,$Y$2:$Z$19,2,FALSE)),H2,VLOOKUP(B2,$Y$2:$Z$19,2,FALSE))</f>
+        <f>IF(ISNA(VLOOKUP(B2,$Y$2:$Z$26,2,FALSE)),H2,VLOOKUP(B2,$Y$2:$Z$26,2,FALSE))</f>
         <v>47.922183194688699</v>
       </c>
       <c r="J2">
@@ -2745,7 +2738,7 @@
       </c>
       <c r="W2">
         <f>SUM(N:N)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y2" t="s">
         <v>266</v>
@@ -2786,7 +2779,7 @@
         <v>43.659935667633398</v>
       </c>
       <c r="I3" s="4">
-        <f t="shared" ref="I3:I66" si="3">IF(ISNA(VLOOKUP(B3,$Y$2:$Z$19,2,FALSE)),H3,VLOOKUP(B3,$Y$2:$Z$19,2,FALSE))</f>
+        <f t="shared" ref="I3:I66" si="3">IF(ISNA(VLOOKUP(B3,$Y$2:$Z$26,2,FALSE)),H3,VLOOKUP(B3,$Y$2:$Z$26,2,FALSE))</f>
         <v>43.659935667633398</v>
       </c>
       <c r="J3">
@@ -2835,7 +2828,7 @@
       </c>
       <c r="W3">
         <f>SUM(O:O)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y3" t="s">
         <v>330</v>
@@ -2919,7 +2912,7 @@
       </c>
       <c r="W4">
         <f>SUM(P:P)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y4" t="s">
         <v>105</v>
@@ -2997,7 +2990,7 @@
       </c>
       <c r="W5">
         <f>SUM(Q:Q)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y5" t="s">
         <v>78</v>
@@ -3233,7 +3226,7 @@
       </c>
       <c r="W8">
         <f>W3+W4+W5</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="Y8" t="s">
         <v>331</v>
@@ -3430,15 +3423,15 @@
         <v>38.465307116646301</v>
       </c>
       <c r="J11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K11">
         <f t="shared" si="4"/>
-        <v>38.465307116646301</v>
+        <v>0</v>
       </c>
       <c r="L11">
         <f t="shared" si="0"/>
-        <v>8600</v>
+        <v>0</v>
       </c>
       <c r="M11">
         <f t="shared" si="1"/>
@@ -3458,7 +3451,7 @@
       </c>
       <c r="Q11">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R11">
         <f t="shared" si="5"/>
@@ -3616,7 +3609,7 @@
       <c r="V13" s="2"/>
       <c r="W13" s="2"/>
       <c r="Y13" s="13" t="s">
-        <v>320</v>
+        <v>261</v>
       </c>
       <c r="Z13" s="13"/>
       <c r="AA13" s="13"/>
@@ -3651,7 +3644,7 @@
       </c>
       <c r="I14" s="4">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>34.886217090854103</v>
       </c>
       <c r="J14">
         <v>0</v>
@@ -3686,13 +3679,13 @@
       </c>
       <c r="R14">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>4.4159768469435576</v>
       </c>
       <c r="T14" s="2" t="s">
         <v>26</v>
       </c>
       <c r="Y14" s="13" t="s">
-        <v>431</v>
+        <v>320</v>
       </c>
     </row>
     <row r="15" spans="1:27" x14ac:dyDescent="0.45">
@@ -3728,19 +3721,19 @@
         <v>36.903240854862702</v>
       </c>
       <c r="J15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K15">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>36.903240854862702</v>
       </c>
       <c r="L15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>7800</v>
       </c>
       <c r="M15">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N15">
         <f t="shared" si="6"/>
@@ -3762,6 +3755,7 @@
         <f t="shared" si="5"/>
         <v>4.7311847249823975</v>
       </c>
+      <c r="Y15" s="13"/>
     </row>
     <row r="16" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
@@ -3830,8 +3824,17 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="Y16" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z16">
+        <v>0</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -3898,8 +3901,11 @@
         <f t="shared" si="5"/>
         <v>3.8593707028017761</v>
       </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="Y17" s="13" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -3966,8 +3972,11 @@
         <f t="shared" si="5"/>
         <v>4.5558719188829064</v>
       </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="Y18" s="13" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>5</v>
       </c>
@@ -4034,8 +4043,11 @@
         <f t="shared" si="5"/>
         <v>4.0808428241939865</v>
       </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="Y19" s="13" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -4102,11 +4114,14 @@
         <f t="shared" si="5"/>
         <v>4.3652398505355476</v>
       </c>
-      <c r="T20" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="Y20" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="Z20">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>5</v>
       </c>
@@ -4173,11 +4188,8 @@
         <f t="shared" si="5"/>
         <v>4.1655143668738113</v>
       </c>
-      <c r="T21" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.45">
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -4244,11 +4256,8 @@
         <f t="shared" si="5"/>
         <v>4.1918658169937162</v>
       </c>
-      <c r="T22" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.45">
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -4315,11 +4324,8 @@
         <f t="shared" si="5"/>
         <v>4.3659725627470269</v>
       </c>
-      <c r="T23" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.45">
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -4387,7 +4393,7 @@
         <v>4.058633360190397</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>6</v>
       </c>
@@ -4455,7 +4461,7 @@
         <v>4.1065815528385068</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -4523,7 +4529,7 @@
         <v>3.9573427854017229</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>8</v>
       </c>
@@ -4590,8 +4596,11 @@
         <f t="shared" si="5"/>
         <v>3.9728078173542225</v>
       </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="T27" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -4621,18 +4630,18 @@
       </c>
       <c r="I28" s="4">
         <f t="shared" si="3"/>
-        <v>39.236745245287402</v>
+        <v>0</v>
       </c>
       <c r="J28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K28">
         <f t="shared" si="4"/>
-        <v>39.236745245287402</v>
+        <v>0</v>
       </c>
       <c r="L28">
         <f t="shared" si="0"/>
-        <v>7200</v>
+        <v>0</v>
       </c>
       <c r="M28">
         <f t="shared" si="7"/>
@@ -4644,7 +4653,7 @@
       </c>
       <c r="O28">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P28">
         <f t="shared" si="7"/>
@@ -4656,10 +4665,13 @@
       </c>
       <c r="R28">
         <f t="shared" si="5"/>
-        <v>5.4495479507343614</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+      <c r="T28" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>5</v>
       </c>
@@ -4726,8 +4738,11 @@
         <f t="shared" si="5"/>
         <v>4.0989916133222364</v>
       </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="T29" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>9</v>
       </c>
@@ -4794,8 +4809,11 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.45">
+      <c r="T30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>5</v>
       </c>
@@ -4863,7 +4881,7 @@
         <v>3.2750780125281969</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>6</v>
       </c>
@@ -6052,15 +6070,15 @@
         <v>31.1666666666666</v>
       </c>
       <c r="J49">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K49">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>31.1666666666666</v>
       </c>
       <c r="L49">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6200</v>
       </c>
       <c r="M49">
         <f t="shared" si="9"/>
@@ -6068,7 +6086,7 @@
       </c>
       <c r="N49">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O49">
         <f t="shared" si="9"/>
@@ -7272,7 +7290,7 @@
         <v>25.145508256983302</v>
       </c>
       <c r="I67" s="4">
-        <f t="shared" ref="I67:I130" si="14">IF(ISNA(VLOOKUP(B67,$Y$2:$Z$19,2,FALSE)),H67,VLOOKUP(B67,$Y$2:$Z$19,2,FALSE))</f>
+        <f t="shared" ref="I67:I130" si="14">IF(ISNA(VLOOKUP(B67,$Y$2:$Z$26,2,FALSE)),H67,VLOOKUP(B67,$Y$2:$Z$26,2,FALSE))</f>
         <v>25.145508256983302</v>
       </c>
       <c r="J67">
@@ -7409,18 +7427,18 @@
       </c>
       <c r="I69" s="4">
         <f t="shared" si="14"/>
-        <v>22.284179072180699</v>
+        <v>26</v>
       </c>
       <c r="J69">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K69">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="L69">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>5100</v>
       </c>
       <c r="M69">
         <f t="shared" si="11"/>
@@ -7436,7 +7454,7 @@
       </c>
       <c r="P69">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q69">
         <f t="shared" si="11"/>
@@ -7444,7 +7462,7 @@
       </c>
       <c r="R69">
         <f t="shared" si="16"/>
-        <v>4.3694468768981762</v>
+        <v>5.098039215686275</v>
       </c>
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.45">
@@ -7616,15 +7634,15 @@
         <v>26.086673839399602</v>
       </c>
       <c r="J72">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K72">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>26.086673839399602</v>
       </c>
       <c r="L72">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>5100</v>
       </c>
       <c r="M72">
         <f t="shared" ref="M72:Q81" si="17">$J72*IF($A72=M$1,1,0)</f>
@@ -7632,7 +7650,7 @@
       </c>
       <c r="N72">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O72">
         <f t="shared" si="17"/>
@@ -8089,7 +8107,7 @@
       </c>
       <c r="I79" s="4">
         <f t="shared" si="14"/>
-        <v>23.996417164128601</v>
+        <v>0</v>
       </c>
       <c r="J79">
         <v>0</v>
@@ -8124,7 +8142,7 @@
       </c>
       <c r="R79">
         <f t="shared" si="16"/>
-        <v>4.8972279926793068</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.45">
@@ -8905,18 +8923,18 @@
       </c>
       <c r="I91" s="4">
         <f t="shared" si="14"/>
-        <v>25.715934117837801</v>
+        <v>0</v>
       </c>
       <c r="J91">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K91">
         <f t="shared" si="15"/>
-        <v>25.715934117837801</v>
+        <v>0</v>
       </c>
       <c r="L91">
         <f t="shared" si="12"/>
-        <v>4600</v>
+        <v>0</v>
       </c>
       <c r="M91">
         <f t="shared" si="18"/>
@@ -8924,7 +8942,7 @@
       </c>
       <c r="N91">
         <f t="shared" si="18"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O91">
         <f t="shared" si="18"/>
@@ -8940,7 +8958,7 @@
       </c>
       <c r="R91">
         <f t="shared" si="16"/>
-        <v>5.590420460399522</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:18" x14ac:dyDescent="0.45">
@@ -10132,15 +10150,15 @@
         <v>22.358930145420899</v>
       </c>
       <c r="J109">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K109">
         <f t="shared" si="15"/>
-        <v>22.358930145420899</v>
+        <v>0</v>
       </c>
       <c r="L109">
         <f t="shared" si="12"/>
-        <v>4200</v>
+        <v>0</v>
       </c>
       <c r="M109">
         <f t="shared" si="20"/>
@@ -10152,7 +10170,7 @@
       </c>
       <c r="O109">
         <f t="shared" si="20"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P109">
         <f t="shared" si="20"/>
@@ -11489,7 +11507,7 @@
       </c>
       <c r="I129" s="4">
         <f t="shared" si="14"/>
-        <v>19.878082396425199</v>
+        <v>0</v>
       </c>
       <c r="J129">
         <v>0</v>
@@ -11524,7 +11542,7 @@
       </c>
       <c r="R129">
         <f t="shared" si="16"/>
-        <v>5.5216895545625553</v>
+        <v>0</v>
       </c>
     </row>
     <row r="130" spans="1:18" x14ac:dyDescent="0.45">
@@ -11624,7 +11642,7 @@
         <v>14.621811992703099</v>
       </c>
       <c r="I131" s="4">
-        <f t="shared" ref="I131:I194" si="25">IF(ISNA(VLOOKUP(B131,$Y$2:$Z$19,2,FALSE)),H131,VLOOKUP(B131,$Y$2:$Z$19,2,FALSE))</f>
+        <f t="shared" ref="I131:I194" si="25">IF(ISNA(VLOOKUP(B131,$Y$2:$Z$26,2,FALSE)),H131,VLOOKUP(B131,$Y$2:$Z$26,2,FALSE))</f>
         <v>14.621811992703099</v>
       </c>
       <c r="J131">
@@ -11832,15 +11850,15 @@
         <v>21.170286284777301</v>
       </c>
       <c r="J134">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K134">
         <f t="shared" si="26"/>
-        <v>0</v>
+        <v>21.170286284777301</v>
       </c>
       <c r="L134">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>3500</v>
       </c>
       <c r="M134">
         <f t="shared" si="28"/>
@@ -11852,7 +11870,7 @@
       </c>
       <c r="O134">
         <f t="shared" si="28"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P134">
         <f t="shared" si="28"/>
@@ -13257,22 +13275,22 @@
       </c>
       <c r="I155" s="4">
         <f t="shared" si="25"/>
-        <v>21.738903022030598</v>
+        <v>0</v>
       </c>
       <c r="J155">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K155">
         <f t="shared" si="26"/>
-        <v>21.738903022030598</v>
+        <v>0</v>
       </c>
       <c r="L155">
         <f t="shared" si="23"/>
-        <v>3100</v>
+        <v>0</v>
       </c>
       <c r="M155">
         <f t="shared" si="30"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N155">
         <f t="shared" si="30"/>
@@ -13292,7 +13310,7 @@
       </c>
       <c r="R155">
         <f t="shared" si="27"/>
-        <v>7.0125493619453545</v>
+        <v>0</v>
       </c>
     </row>
     <row r="156" spans="1:18" x14ac:dyDescent="0.45">
@@ -15976,7 +15994,7 @@
         <v>4.3620815670223596</v>
       </c>
       <c r="I195" s="4">
-        <f t="shared" ref="I195:I258" si="37">IF(ISNA(VLOOKUP(B195,$Y$2:$Z$19,2,FALSE)),H195,VLOOKUP(B195,$Y$2:$Z$19,2,FALSE))</f>
+        <f t="shared" ref="I195:I258" si="37">IF(ISNA(VLOOKUP(B195,$Y$2:$Z$26,2,FALSE)),H195,VLOOKUP(B195,$Y$2:$Z$26,2,FALSE))</f>
         <v>4.3620815670223596</v>
       </c>
       <c r="J195">
@@ -19611,7 +19629,7 @@
         <v>0</v>
       </c>
       <c r="I259" s="4">
-        <f t="shared" ref="I259:I279" si="44">IF(ISNA(VLOOKUP(B259,$Y$2:$Z$19,2,FALSE)),H259,VLOOKUP(B259,$Y$2:$Z$19,2,FALSE))</f>
+        <f t="shared" ref="I259:I279" si="44">IF(ISNA(VLOOKUP(B259,$Y$2:$Z$26,2,FALSE)),H259,VLOOKUP(B259,$Y$2:$Z$26,2,FALSE))</f>
         <v>0</v>
       </c>
       <c r="R259">
@@ -20604,12 +20622,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="E3:E104 A2:D104 E2:R2 A197:E300 J3:Q235 R3:R279 F3:I279">
-    <cfRule type="expression" dxfId="7" priority="2">
+    <cfRule type="expression" dxfId="6" priority="2">
       <formula>$J2=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A105:E196">
-    <cfRule type="expression" dxfId="6" priority="1">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>$J105=1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -24237,27 +24255,27 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="expression" dxfId="5" priority="5">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>$I2=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3">
-    <cfRule type="expression" dxfId="4" priority="4">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>$I3=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="expression" dxfId="3" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>$I4=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>$I5=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$I6=1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>